<commit_message>
:arrow_up: Update to Python 3.11 kernel, remove engarde
</commit_message>
<xml_diff>
--- a/docs/data-processing/serialisation-formats/library.xlsx
+++ b/docs/data-processing/serialisation-formats/library.xlsx
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>License</t>
-  </si>
-  <si>
-    <t>Publication date</t>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Sprache</t>
+  </si>
+  <si>
+    <t>Autor*innen</t>
+  </si>
+  <si>
+    <t>Lizenz</t>
+  </si>
+  <si>
+    <t>Veröffentlichungsdatum</t>
   </si>
   <si>
     <t>Python basics</t>
@@ -204,19 +204,19 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -388,9 +388,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -470,7 +470,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -498,10 +498,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -757,9 +757,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
+              <a:alpha val="38000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1047,7 +1047,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1075,10 +1075,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>